<commit_message>
major fix in parsing schedule
</commit_message>
<xml_diff>
--- a/api/ConstraintModel/formatted_schedule.xlsx
+++ b/api/ConstraintModel/formatted_schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="306">
   <si>
     <t>FIRST</t>
   </si>
@@ -125,8 +125,11 @@
   </si>
   <si>
     <t xml:space="preserve">(0, 'theory of computation', 'small_lec', '5 csen ii', 53)
-(0, 'graphics', 'lab', '5 csen ii 23', 63)
-(0, 'data bases', 'lab', '5 csen ii 22', 62)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0, 'graphics', 'lab', '5 dmet 23', 63)
+(0, 'data bases', 'lab', '5 dmet 22', 62)
 </t>
   </si>
   <si>
@@ -190,8 +193,11 @@
 (1, 'comm ne', 'tut', '5 csen ii 19', 36)
 (1, 'math', 'tut', '5 csen ii 20', 35)
 (1, 'data bases', 'lab', '5 csen ii 21', 63)
-(1, 'math', 'tut', '5 csen ii 23', 34)
-(1, 'data bases', 'tut', '5 csen ii 22', 33)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, 'math', 'tut', '5 dmet 23', 34)
+(1, 'data bases', 'tut', '5 dmet 22', 33)
 </t>
   </si>
   <si>
@@ -259,7 +265,10 @@
     <t xml:space="preserve">(2, 'theory of computation', 'tut', '5 csen ii 21', 31)
 (2, 'medi', 'tut', '5 csen ii 19', 30)
 (2, 'math', 'tut', '5 csen ii 16', 29)
-(2, 'computer graphics', 'small_lec', '5 csen ii', 52)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, 'computer graphics', 'small_lec', '5 dmet', 52)
 </t>
   </si>
   <si>
@@ -328,7 +337,10 @@
 (3, 'comm ne', 'tut', '5 csen ii 21', 35)
 (3, 'medi', 'tut', '5 csen ii 16', 34)
 (3, 'dsd', 'tut', '5 csen ii 20', 33)
-(3, 'graphics', 'tut', '5 csen ii 23', 32)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3, 'graphics', 'tut', '5 dmet 23', 32)
 </t>
   </si>
   <si>
@@ -425,8 +437,11 @@
 (5, 'data bases', 'lab', '5 csen ii 19', 60)
 (5, 'dsd', 'tut', '5 csen ii 21', 34)
 (5, 'theory of computation', 'tut', '5 csen ii 16', 33)
-(5, 'comm ne', 'tut', '5 csen ii 23', 32)
-(5, 'graphics', 'lab', '5 csen ii 22', 59)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5, 'comm ne', 'tut', '5 dmet 23', 32)
+(5, 'graphics', 'lab', '5 dmet 22', 59)
 </t>
   </si>
   <si>
@@ -627,8 +642,11 @@
 (8, 'comm ne', 'tut', '5 csen ii 18', 34)
 (8, 'theory of computation', 'tut', '5 csen ii 19', 33)
 (8, 'comm ne', 'tut', '5 csen ii 16', 32)
-(8, 'medi', 'tut', '5 csen ii 23', 31)
-(8, 'dsd', 'tut', '5 csen ii 22', 30)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8, 'medi', 'tut', '5 dmet 23', 31)
+(8, 'dsd', 'tut', '5 dmet 22', 30)
 </t>
   </si>
   <si>
@@ -705,8 +723,11 @@
   </si>
   <si>
     <t xml:space="preserve">(10, 'theory of computation', 'small_lec', '5 csen ii', 52)
-(10, 'data bases', 'tut', '5 csen ii 23', 36)
-(10, 'math', 'tut', '5 csen ii 22', 35)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(10, 'data bases', 'tut', '5 dmet 23', 36)
+(10, 'math', 'tut', '5 dmet 22', 35)
 </t>
   </si>
   <si>
@@ -816,8 +837,11 @@
 (12, 'math', 'tut', '5 csen ii 17', 30)
 (12, 'math', 'tut', '5 csen ii 19', 29)
 (12, 'data bases', 'lab', '5 csen ii 18', 59)
-(12, 'dsd', 'tut', '5 csen ii 23', 28)
-(12, 'medi', 'tut', '5 csen ii 22', 27)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(12, 'dsd', 'tut', '5 dmet 23', 28)
+(12, 'medi', 'tut', '5 dmet 22', 27)
 </t>
   </si>
   <si>
@@ -878,8 +902,11 @@
 (13, 'medi', 'tut', '5 csen ii 21', 25)
 (13, 'math', 'tut', '5 csen ii 18', 24)
 (13, 'data bases', 'tut', '5 csen ii 17', 23)
-(13, 'data bases', 'lab', '5 csen ii 23', 56)
-(13, 'comm ne', 'tut', '5 csen ii 22', 22)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(13, 'data bases', 'lab', '5 dmet 23', 56)
+(13, 'comm ne', 'tut', '5 dmet 22', 22)
 </t>
   </si>
   <si>
@@ -2132,13 +2159,13 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2146,10 +2173,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2160,16 +2187,16 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2177,16 +2204,16 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2194,10 +2221,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2208,13 +2235,13 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2225,7 +2252,7 @@
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2233,10 +2260,10 @@
         <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2254,16 +2281,16 @@
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2274,13 +2301,13 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2291,38 +2318,50 @@
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2330,19 +2369,19 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2350,16 +2389,16 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2404,16 +2443,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2421,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2439,16 +2478,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2456,19 +2495,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2476,13 +2515,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2490,16 +2529,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2507,10 +2546,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2518,13 +2557,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2532,19 +2571,19 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2552,16 +2591,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2569,16 +2608,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2586,19 +2625,19 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2606,34 +2645,40 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -2680,16 +2725,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2697,13 +2742,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2711,16 +2756,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2728,10 +2773,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2769,16 +2814,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2786,16 +2831,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2803,16 +2848,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2820,16 +2865,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2837,34 +2882,43 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -2911,19 +2965,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2931,13 +2985,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2945,19 +2999,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2965,13 +3019,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="F5" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3009,16 +3063,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3026,16 +3080,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3043,16 +3097,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3075,16 +3129,16 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3092,16 +3146,16 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3109,13 +3163,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3170,19 +3224,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="F4" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3190,7 +3244,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3198,16 +3252,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3215,19 +3269,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="F7" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3235,10 +3289,10 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3246,19 +3300,19 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3266,10 +3320,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3277,7 +3331,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3285,19 +3339,19 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="F12" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3305,16 +3359,16 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="F13" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3322,16 +3376,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3354,19 +3408,19 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="F18" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3374,19 +3428,19 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3394,13 +3448,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3445,19 +3499,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3465,7 +3519,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3483,19 +3537,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="F6" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3503,16 +3557,16 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3520,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3528,16 +3582,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3545,10 +3599,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3556,10 +3610,10 @@
         <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3567,16 +3621,16 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="F12" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3584,16 +3638,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3606,13 +3660,13 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3620,13 +3674,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3634,7 +3688,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3642,16 +3696,16 @@
         <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="F18" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3659,16 +3713,16 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3676,16 +3730,16 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>